<commit_message>
there is a bug in the generation of the dancer array
</commit_message>
<xml_diff>
--- a/22-23_ALL_PEOPLE_INVOLVED.xlsx
+++ b/22-23_ALL_PEOPLE_INVOLVED.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jacob\Documents\Barrio\BarrioGreenRoom\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E6F15A8-DF67-4C1D-97AF-6732200A1E65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6859758-FEFE-4777-8556-E21D2EA8A15F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10245" yWindow="0" windowWidth="10245" windowHeight="10920" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5115" yWindow="0" windowWidth="15375" windowHeight="10920" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="All" sheetId="1" r:id="rId1"/>
@@ -20993,7 +20993,7 @@
   </sheetPr>
   <dimension ref="A1:M1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
@@ -25697,8 +25697,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45DDC02B-722C-4673-B4D9-B206197E0872}">
   <dimension ref="A1:B21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Good enough state for me
</commit_message>
<xml_diff>
--- a/22-23_ALL_PEOPLE_INVOLVED.xlsx
+++ b/22-23_ALL_PEOPLE_INVOLVED.xlsx
@@ -8,17 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jacob\Documents\Barrio\BarrioGreenRoom\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6859758-FEFE-4777-8556-E21D2EA8A15F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E1E5782-C704-4BF9-8AF3-E4D5905E69C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5115" yWindow="0" windowWidth="15375" windowHeight="10920" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10245" yWindow="0" windowWidth="10245" windowHeight="10920" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="All" sheetId="1" r:id="rId1"/>
     <sheet name="Committees" sheetId="2" r:id="rId2"/>
     <sheet name="Dances" sheetId="3" r:id="rId3"/>
     <sheet name="Cast" sheetId="6" r:id="rId4"/>
-    <sheet name="FISDU Seniors" sheetId="4" r:id="rId5"/>
-    <sheet name="Other" sheetId="5" r:id="rId6"/>
+    <sheet name="Props" sheetId="7" r:id="rId5"/>
+    <sheet name="FISDU Seniors" sheetId="4" r:id="rId6"/>
+    <sheet name="Other" sheetId="5" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">All!$D$1:$D$989</definedName>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="669" uniqueCount="365">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="681" uniqueCount="367">
   <si>
     <t>First Name</t>
   </si>
@@ -1123,6 +1124,12 @@
   </si>
   <si>
     <t>benilde</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kai </t>
+  </si>
+  <si>
+    <t>Natasha</t>
   </si>
 </sst>
 </file>
@@ -1513,7 +1520,7 @@
   <dimension ref="A1:K989"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B36" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B58" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="B55" sqref="B55"/>
@@ -25697,7 +25704,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45DDC02B-722C-4673-B4D9-B206197E0872}">
   <dimension ref="A1:B21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
@@ -25882,6 +25889,81 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC0B1C43-7B21-4B4B-9DBE-B70D41F194DB}">
+  <dimension ref="A1:A12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>217</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -26164,7 +26246,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>

</xml_diff>